<commit_message>
removal of PII 2
</commit_message>
<xml_diff>
--- a/input/save_the_date_test.xlsx
+++ b/input/save_the_date_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\projectWAmsg\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A1B727-B370-4285-AA99-84C982105A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1EAC0-E3DA-4CF2-B0E0-B2F4BF080374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{B7C1674E-305B-44C3-94F6-03CD71764A58}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
-  <si>
-    <t>+6584992114</t>
-  </si>
-  <si>
-    <t>+6581572813</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>number</t>
   </si>
@@ -50,43 +44,13 @@
     <t>img_path</t>
   </si>
   <si>
-    <t>./input/KWY_save_the_date.png</t>
-  </si>
-  <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>Baby</t>
   </si>
   <si>
     <t>opening_msg</t>
   </si>
   <si>
     <t>closing_msg</t>
-  </si>
-  <si>
-    <t>This is a test save the date msg :)</t>
-  </si>
-  <si>
-    <t>Hello! Walala</t>
-  </si>
-  <si>
-    <t>Hello!</t>
-  </si>
-  <si>
-    <t>+6587589669</t>
-  </si>
-  <si>
-    <t>Hello Boss</t>
-  </si>
-  <si>
-    <t>Handsome Kent</t>
-  </si>
-  <si>
-    <t>Can you see me &lt;3</t>
   </si>
 </sst>
 </file>
@@ -439,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3637F3-E035-4AF5-B9F5-82C0D33EFC32}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,67 +418,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -523,20 +439,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9a00c2e3-f6ad-41ac-b5ae-b18dddc68917" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9a00c2e3-f6ad-41ac-b5ae-b18dddc68917" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -749,6 +665,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1C5865A-E95B-42A1-9A96-D1503AB0D086}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68BBEF07-7187-48BE-B47D-77E4E8E7BBF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -761,14 +685,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="3267d801-ab2e-47a4-b909-25d670dcad83"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1C5865A-E95B-42A1-9A96-D1503AB0D086}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>